<commit_message>
Añadimos imagenes + cambio a rutas relativas para auditoria
</commit_message>
<xml_diff>
--- a/TiendaProyecto/datos_exportados.xlsx
+++ b/TiendaProyecto/datos_exportados.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>ID_Videojuego</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>Nintendo NES</t>
+  </si>
+  <si>
+    <t>Zelda Remastered</t>
+  </si>
+  <si>
+    <t>Nintendo Switch</t>
   </si>
   <si>
     <t>Super Mario Bros 3</t>
@@ -161,7 +167,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -271,33 +277,33 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>547.0</v>
+        <v>347.0</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" t="n">
-        <v>1000.0</v>
+        <v>500.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>554.0</v>
+        <v>547.0</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>87.0</v>
+        <v>1000.0</v>
       </c>
       <c r="E8" t="n">
         <v>2.0</v>
@@ -305,7 +311,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>555.0</v>
+        <v>554.0</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -314,21 +320,21 @@
         <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>65.0</v>
+        <v>87.0</v>
       </c>
       <c r="E9" t="n">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>556.0</v>
+        <v>555.0</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D10" t="n">
         <v>65.0</v>
@@ -339,44 +345,44 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>4467.0</v>
+        <v>556.0</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
       <c r="D11" t="n">
-        <v>15.5</v>
+        <v>65.0</v>
       </c>
       <c r="E11" t="n">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9002.0</v>
+        <v>4467.0</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D12" t="n">
-        <v>54.0</v>
+        <v>15.5</v>
       </c>
       <c r="E12" t="n">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>9003.0</v>
+        <v>9002.0</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -390,16 +396,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>10101.0</v>
+        <v>9003.0</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D14" t="n">
-        <v>99999.0</v>
+        <v>54.0</v>
       </c>
       <c r="E14" t="n">
         <v>1.0</v>
@@ -407,7 +413,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>45484.0</v>
+        <v>10101.0</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
@@ -416,15 +422,15 @@
         <v>28</v>
       </c>
       <c r="D15" t="n">
-        <v>150.0</v>
+        <v>99999.0</v>
       </c>
       <c r="E15" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>88965.0</v>
+        <v>45484.0</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
@@ -433,77 +439,94 @@
         <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>97.0</v>
+        <v>150.0</v>
       </c>
       <c r="E16" t="n">
-        <v>44.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>90909.0</v>
+        <v>88965.0</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="D17" t="n">
-        <v>157.0</v>
+        <v>97.0</v>
       </c>
       <c r="E17" t="n">
-        <v>4.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>99984.0</v>
+        <v>90909.0</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="n">
-        <v>89.0</v>
+        <v>157.0</v>
       </c>
       <c r="E18" t="n">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>121212.0</v>
+        <v>99984.0</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D19" t="n">
-        <v>8888.0</v>
+        <v>89.0</v>
       </c>
       <c r="E19" t="n">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
+        <v>121212.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="n">
+        <v>8888.0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
         <v>9875555.0</v>
       </c>
-      <c r="B20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D21" t="n">
         <v>1600.0</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E21" t="n">
         <v>1.0</v>
       </c>
     </row>

</xml_diff>